<commit_message>
added in the math for price per meter
</commit_message>
<xml_diff>
--- a/LoveCraftTrial.xlsx
+++ b/LoveCraftTrial.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="75">
   <si>
     <t>name</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>price(kinda)</t>
+  </si>
+  <si>
+    <t>ppm</t>
   </si>
   <si>
     <t>Debbie Bliss Donegal Luxury Tweed Aran</t>
@@ -593,13 +596,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,25 +624,28 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G2">
         <v>88</v>
@@ -647,25 +653,28 @@
       <c r="H2">
         <v>8.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>0.09379999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G3">
         <v>180</v>
@@ -673,25 +682,28 @@
       <c r="H3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <v>0.0389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G4">
         <v>880</v>
@@ -699,25 +711,28 @@
       <c r="H4">
         <v>82.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <v>0.09379999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G5">
         <v>200</v>
@@ -725,25 +740,28 @@
       <c r="H5">
         <v>8.49</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <v>0.0425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G6">
         <v>440</v>
@@ -751,25 +769,28 @@
       <c r="H6">
         <v>41.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <v>0.09379999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G7">
         <v>900</v>
@@ -777,25 +798,28 @@
       <c r="H7">
         <v>7.49</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <v>0.0083</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G8">
         <v>166</v>
@@ -803,25 +827,28 @@
       <c r="H8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <v>0.0482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G9">
         <v>90</v>
@@ -829,25 +856,28 @@
       <c r="H9">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <v>0.4444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G10">
         <v>550</v>
@@ -855,25 +885,28 @@
       <c r="H10">
         <v>6.95</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <v>0.0126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G11">
         <v>166</v>
@@ -881,25 +914,28 @@
       <c r="H11">
         <v>9.99</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <v>0.0602</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12">
         <v>1800</v>
@@ -907,25 +943,28 @@
       <c r="H12">
         <v>4.49</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <v>0.0025</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G13">
         <v>166</v>
@@ -933,25 +972,28 @@
       <c r="H13">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <v>0.4819</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G14">
         <v>900</v>
@@ -959,25 +1001,28 @@
       <c r="H14">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <v>0.0077</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G15">
         <v>180</v>
@@ -985,25 +1030,28 @@
       <c r="H15">
         <v>8.699999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <v>0.0483</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G16">
         <v>199</v>
@@ -1011,25 +1059,28 @@
       <c r="H16">
         <v>6.95</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <v>0.0349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G17">
         <v>137</v>
@@ -1037,25 +1088,28 @@
       <c r="H17">
         <v>9.49</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <v>0.0693</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G18">
         <v>166</v>
@@ -1063,25 +1117,28 @@
       <c r="H18">
         <v>3.49</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G19">
         <v>87</v>
@@ -1089,25 +1146,28 @@
       <c r="H19">
         <v>9.99</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <v>0.1148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G20">
         <v>300</v>
@@ -1115,25 +1175,28 @@
       <c r="H20">
         <v>8.49</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <v>0.0283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G21">
         <v>166</v>
@@ -1141,25 +1204,28 @@
       <c r="H21">
         <v>9.49</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <v>0.0572</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G22">
         <v>100</v>
@@ -1167,25 +1233,28 @@
       <c r="H22">
         <v>12.99</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <v>0.1299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G23">
         <v>200</v>
@@ -1193,25 +1262,28 @@
       <c r="H23">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G24">
         <v>140</v>
@@ -1219,31 +1291,37 @@
       <c r="H24">
         <v>6.25</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <v>0.0446</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G25">
         <v>166</v>
       </c>
       <c r="H25">
         <v>9.99</v>
+      </c>
+      <c r="I25">
+        <v>0.0602</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made it to 4 dp instead of 2
all good however think there is an issue with the list of prices most of them match but not all??
</commit_message>
<xml_diff>
--- a/LoveCraftTrial.xlsx
+++ b/LoveCraftTrial.xlsx
@@ -245,6 +245,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -297,8 +300,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -601,35 +605,38 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="9" max="9" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -653,12 +660,12 @@
       <c r="H2">
         <v>8.25</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>0.09379999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -682,12 +689,12 @@
       <c r="H3">
         <v>7</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>0.0389</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -711,12 +718,12 @@
       <c r="H4">
         <v>82.5</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>0.09379999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -740,12 +747,12 @@
       <c r="H5">
         <v>8.49</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>0.0425</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -769,12 +776,12 @@
       <c r="H6">
         <v>41.25</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>0.09379999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -798,12 +805,12 @@
       <c r="H7">
         <v>7.49</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <v>0.0083</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -827,12 +834,12 @@
       <c r="H8">
         <v>8</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <v>0.0482</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -856,12 +863,12 @@
       <c r="H9">
         <v>40</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>0.4444</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -885,12 +892,12 @@
       <c r="H10">
         <v>6.95</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <v>0.0126</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -914,12 +921,12 @@
       <c r="H11">
         <v>9.99</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>0.0602</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -943,12 +950,12 @@
       <c r="H12">
         <v>4.49</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="1">
         <v>0.0025</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -972,12 +979,12 @@
       <c r="H13">
         <v>80</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <v>0.4819</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -1001,12 +1008,12 @@
       <c r="H14">
         <v>6.9</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="1">
         <v>0.0077</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -1030,12 +1037,12 @@
       <c r="H15">
         <v>8.699999999999999</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="1">
         <v>0.0483</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -1059,12 +1066,12 @@
       <c r="H16">
         <v>6.95</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="1">
         <v>0.0349</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -1088,12 +1095,12 @@
       <c r="H17">
         <v>9.49</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="1">
         <v>0.0693</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -1117,12 +1124,12 @@
       <c r="H18">
         <v>3.49</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
         <v>0.021</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -1146,12 +1153,12 @@
       <c r="H19">
         <v>9.99</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="1">
         <v>0.1148</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -1175,12 +1182,12 @@
       <c r="H20">
         <v>8.49</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="1">
         <v>0.0283</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -1204,12 +1211,12 @@
       <c r="H21">
         <v>9.49</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="1">
         <v>0.0572</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -1233,12 +1240,12 @@
       <c r="H22">
         <v>12.99</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="1">
         <v>0.1299</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -1262,12 +1269,12 @@
       <c r="H23">
         <v>28</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="1">
         <v>0.14</v>
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -1291,12 +1298,12 @@
       <c r="H24">
         <v>6.25</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="1">
         <v>0.0446</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -1320,7 +1327,7 @@
       <c r="H25">
         <v>9.99</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="1">
         <v>0.0602</v>
       </c>
     </row>

</xml_diff>